<commit_message>
modified pom.xml to import execution implementatio 'wq' is not recognized as an internal or external command, operable program or batch file.
</commit_message>
<xml_diff>
--- a/fuse-brms-decisiontable-poc.rules/src/main/resources/data/product_role_mapping.xlsx
+++ b/fuse-brms-decisiontable-poc.rules/src/main/resources/data/product_role_mapping.xlsx
@@ -276,14 +276,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
   <si>
     <t>RuleSet</t>
   </si>
   <si>
-    <t>Some business rules</t>
-  </si>
-  <si>
     <t>Import</t>
   </si>
   <si>
@@ -305,9 +302,6 @@
     <t>Case</t>
   </si>
   <si>
-    <t>Variables</t>
-  </si>
-  <si>
     <t>ProductType</t>
   </si>
   <si>
@@ -362,28 +356,25 @@
     <t>RuleTable Products to be displayed</t>
   </si>
   <si>
-    <t>ProductDetails</t>
-  </si>
-  <si>
-    <t>productType</t>
-  </si>
-  <si>
     <t>poc.decisiontable.fuse.brms.displayproduct.ProductDetails, poc.decisiontable.fuse.brms.displayproduct.UserDetails</t>
   </si>
   <si>
-    <t>UserDetails</t>
-  </si>
-  <si>
-    <t>userRole</t>
-  </si>
-  <si>
-    <t>setDisplayProduct("$param");</t>
-  </si>
-  <si>
-    <t>poc.decisiontable.fuse.brms.displayproduct.ProductDetails productDetail</t>
-  </si>
-  <si>
-    <t>productDetail</t>
+    <t>poc.decisiontable.fuse.brms.displayproduct</t>
+  </si>
+  <si>
+    <t>product:ProductDetails</t>
+  </si>
+  <si>
+    <t>user:UserDetails</t>
+  </si>
+  <si>
+    <t>product.setDisplayProduct("$param");</t>
+  </si>
+  <si>
+    <t>productType=="$param"</t>
+  </si>
+  <si>
+    <t>userRole=="$param"</t>
   </si>
 </sst>
 </file>
@@ -1064,7 +1055,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1081,27 +1072,27 @@
         <v>0</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D2" s="32"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="33"/>
     </row>
@@ -1114,7 +1105,7 @@
     <row r="5" spans="1:4">
       <c r="A5" s="8"/>
       <c r="B5" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -1122,13 +1113,13 @@
     <row r="6" spans="1:4">
       <c r="A6" s="11"/>
       <c r="B6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>5</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1137,216 +1128,210 @@
         <v>28</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>35</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D7" s="29"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>32</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>10</v>
-      </c>
       <c r="C9" s="19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="21"/>
       <c r="B10" s="22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="21"/>
       <c r="B11" s="25" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="21"/>
       <c r="B12" s="25" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="21"/>
       <c r="B13" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="26" t="s">
-        <v>18</v>
-      </c>
       <c r="D13" s="24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="21"/>
       <c r="B14" s="25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="21"/>
       <c r="B15" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="26" t="s">
-        <v>21</v>
-      </c>
       <c r="D15" s="24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="21"/>
       <c r="B16" s="25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="21"/>
       <c r="B17" s="25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="21"/>
       <c r="B18" s="25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="21"/>
       <c r="B19" s="25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="21"/>
       <c r="B20" s="25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="21"/>
       <c r="B21" s="25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="21"/>
       <c r="B22" s="25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="21"/>
       <c r="B23" s="25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="25" spans="1:4" ht="15.75" thickBot="1">
-      <c r="B25" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="28" t="s">
-        <v>34</v>
-      </c>
+      <c r="B25" s="27"/>
+      <c r="C25" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>